<commit_message>
updated reads from trim galore fastqc
</commit_message>
<xml_diff>
--- a/fastqc_reads.xlsx
+++ b/fastqc_reads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/vianaj-genomics-brain-development/MATRICS/aggression_RRBS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9DCBA96-4B2A-2141-BECD-E1FA775DD05F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93839806-7BD1-F145-A08E-60DB141BF6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{023BD309-2127-4947-A528-0CDA9D84BB73}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14540" xr2:uid="{023BD309-2127-4947-A528-0CDA9D84BB73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Filename</t>
   </si>
@@ -68,9 +68,6 @@
     <t>2536_BLB10ACC_r1.fq</t>
   </si>
   <si>
-    <t>2536_BLB11ACC_r1.fq</t>
-  </si>
-  <si>
     <t>2536_BLB01MCC_r1.fq</t>
   </si>
   <si>
@@ -132,16 +129,32 @@
   </si>
   <si>
     <t>2536_BLB10VMH_r1.fq</t>
+  </si>
+  <si>
+    <t>raw data fastqc</t>
+  </si>
+  <si>
+    <t>trim galore fastqc</t>
+  </si>
+  <si>
+    <t>2536_BLB11VMH_r1.fq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,8 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,276 +497,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15164E7D-EBD1-EA4D-A9B8-F95DDCBC446E}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>32734875</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>32199711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>44548525</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>44235205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>36157124</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>35656479</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>34250960</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>34045832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>27016057</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>26738571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>46850517</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>45433468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>15623170</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>15365036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>23655799</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>23535898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>13101162</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>12782594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>24961063</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>24655684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>39956649</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>27367609</v>
+      </c>
+      <c r="C12">
+        <v>26869820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>27367609</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16812862</v>
+      </c>
+      <c r="C13">
+        <v>16345766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>16812862</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25592711</v>
+      </c>
+      <c r="C14">
+        <v>25387628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>25592711</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22428259</v>
+      </c>
+      <c r="C15">
+        <v>22213151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>22428259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22802139</v>
+      </c>
+      <c r="C16">
+        <v>22465755</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>22802139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38287252</v>
+      </c>
+      <c r="C17">
+        <v>36939954</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>38287252</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19188179</v>
+      </c>
+      <c r="C18" s="1">
+        <v>19039160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>19188179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30158648</v>
+      </c>
+      <c r="C19">
+        <v>29892525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>30158648</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21760536</v>
+      </c>
+      <c r="C20">
+        <v>21620848</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>21760536</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25480255</v>
+      </c>
+      <c r="C21">
+        <v>24766166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>25480255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>39956649</v>
+      </c>
+      <c r="C22">
+        <v>36359217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>24638802</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15535422</v>
+      </c>
+      <c r="C23">
+        <v>15269064</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>15535422</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22111183</v>
+      </c>
+      <c r="C24">
+        <v>21414984</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>22111183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29156878</v>
+      </c>
+      <c r="C25">
+        <v>28936004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>29156878</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22864386</v>
+      </c>
+      <c r="C26">
+        <v>22598492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>22864386</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19973971</v>
+      </c>
+      <c r="C27">
+        <v>19524250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>19973971</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42367225</v>
+      </c>
+      <c r="C28">
+        <v>36065618</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>42367225</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>34474341</v>
+      </c>
+      <c r="C29">
+        <v>34039803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>34474341</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18207338</v>
+      </c>
+      <c r="C30">
+        <v>17638909</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>18207338</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25989324</v>
+      </c>
+      <c r="C31">
+        <v>25835203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
-        <v>25989324</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11523057</v>
+      </c>
+      <c r="C32">
+        <v>11129988</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>11523057</v>
+        <v>24638802</v>
+      </c>
+      <c r="C33">
+        <v>23835493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>